<commit_message>
file upload and excell some error solved
</commit_message>
<xml_diff>
--- a/dummy_data/week2.xlsx
+++ b/dummy_data/week2.xlsx
@@ -30,9 +30,6 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Week 1</t>
-  </si>
-  <si>
     <t>Timestamp</t>
   </si>
   <si>
@@ -133,6 +130,9 @@
   </si>
   <si>
     <t>Total Meals</t>
+  </si>
+  <si>
+    <t>Week 2</t>
   </si>
 </sst>
 </file>
@@ -482,123 +482,125 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" customWidth="1"/>
     <col min="11" max="11" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
       <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>13</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>14</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>15</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>16</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>18</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>19</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>20</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>21</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>22</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>23</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>24</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>25</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>26</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>27</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>28</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>29</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>30</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>31</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>32</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>33</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>34</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2">
         <v>30</v>
@@ -703,7 +705,7 @@
     </row>
     <row r="3" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B3" s="2">
         <v>19</v>
@@ -808,7 +810,7 @@
     </row>
     <row r="4" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B4" s="2">
         <v>31</v>
@@ -913,7 +915,7 @@
     </row>
     <row r="5" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B5" s="2">
         <v>26</v>
@@ -1018,7 +1020,7 @@
     </row>
     <row r="6" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B6" s="2">
         <v>20</v>
@@ -1123,7 +1125,7 @@
     </row>
     <row r="7" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B7" s="2">
         <v>8</v>
@@ -1228,7 +1230,7 @@
     </row>
     <row r="8" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B8" s="2">
         <v>13</v>
@@ -1333,7 +1335,7 @@
     </row>
     <row r="9" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B9" s="2">
         <v>17</v>
@@ -1438,7 +1440,7 @@
     </row>
     <row r="10" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B10" s="2">
         <v>5</v>
@@ -1543,7 +1545,7 @@
     </row>
     <row r="11" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B11" s="2">
         <v>6</v>
@@ -1648,7 +1650,7 @@
     </row>
     <row r="12" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B12" s="2">
         <v>11</v>
@@ -1753,7 +1755,7 @@
     </row>
     <row r="13" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B13" s="2">
         <v>24</v>
@@ -1858,7 +1860,7 @@
     </row>
     <row r="14" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B14" s="2">
         <v>12</v>
@@ -1963,7 +1965,7 @@
     </row>
     <row r="15" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B15" s="2">
         <v>16</v>
@@ -2068,7 +2070,7 @@
     </row>
     <row r="16" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B16" s="2">
         <v>29</v>
@@ -2173,7 +2175,7 @@
     </row>
     <row r="17" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B17" s="2">
         <v>14</v>
@@ -2278,7 +2280,7 @@
     </row>
     <row r="18" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B18" s="2">
         <v>15</v>
@@ -2383,7 +2385,7 @@
     </row>
     <row r="19" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B19" s="2">
         <v>71</v>
@@ -2488,7 +2490,7 @@
     </row>
     <row r="20" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B20" s="2">
         <v>27</v>
@@ -2593,7 +2595,7 @@
     </row>
     <row r="21" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B21" s="2">
         <v>91</v>
@@ -2698,7 +2700,7 @@
     </row>
     <row r="22" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B22" s="2">
         <v>3</v>
@@ -2801,7 +2803,7 @@
     </row>
     <row r="23" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B23" s="2">
         <v>9</v>
@@ -2906,7 +2908,7 @@
     </row>
     <row r="24" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B24" s="2">
         <v>7</v>
@@ -3011,7 +3013,7 @@
     </row>
     <row r="25" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B25" s="2">
         <v>82</v>
@@ -3116,7 +3118,7 @@
     </row>
     <row r="26" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B26" s="2">
         <v>22</v>
@@ -3221,7 +3223,7 @@
     </row>
     <row r="27" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B27" s="2">
         <v>4</v>

</xml_diff>

<commit_message>
graph some error solved
</commit_message>
<xml_diff>
--- a/dummy_data/week2.xlsx
+++ b/dummy_data/week2.xlsx
@@ -482,15 +482,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" customWidth="1"/>
-    <col min="7" max="7" width="22.5703125" customWidth="1"/>
     <col min="11" max="11" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>